<commit_message>
hierachy of class and family, processed feedback Kathy
</commit_message>
<xml_diff>
--- a/3_Delete_Attributes_S8.xlsx
+++ b/3_Delete_Attributes_S8.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,20 +459,388 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>S8</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Attribute - Locale</t>
-        </is>
-      </c>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>S8 - Attribute - Locale</t>
+          <t>S</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>